<commit_message>
2. Analyse des performances après 2ème correction
</commit_message>
<xml_diff>
--- a/Analyses/Évolution.xlsx
+++ b/Analyses/Évolution.xlsx
@@ -462,7 +462,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -482,15 +482,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -501,9 +492,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -560,13 +548,34 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -866,7 +875,7 @@
   <dimension ref="A1:M7"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6:D7"/>
+      <selection activeCell="E4" sqref="E4:E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75"/>
@@ -880,88 +889,92 @@
       <c r="A1" s="1"/>
     </row>
     <row r="2" spans="1:13" ht="16.5" thickBot="1">
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="31" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8"/>
-      <c r="G2" s="8"/>
-      <c r="H2" s="8"/>
-      <c r="I2" s="8"/>
-      <c r="J2" s="8"/>
-      <c r="K2" s="8"/>
-      <c r="L2" s="8"/>
-      <c r="M2" s="9"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="32"/>
+      <c r="G2" s="32"/>
+      <c r="H2" s="32"/>
+      <c r="I2" s="32"/>
+      <c r="J2" s="32"/>
+      <c r="K2" s="32"/>
+      <c r="L2" s="32"/>
+      <c r="M2" s="33"/>
     </row>
     <row r="3" spans="1:13" ht="16.5" thickBot="1">
-      <c r="B3" s="20"/>
-      <c r="C3" s="19" t="s">
+      <c r="B3" s="16"/>
+      <c r="C3" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="12" t="s">
+      <c r="D3" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="12" t="s">
+      <c r="E3" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="F3" s="12" t="s">
+      <c r="F3" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="G3" s="12" t="s">
+      <c r="G3" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="H3" s="12" t="s">
+      <c r="H3" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="I3" s="12" t="s">
+      <c r="I3" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="J3" s="12" t="s">
+      <c r="J3" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="K3" s="12" t="s">
+      <c r="K3" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="L3" s="12" t="s">
+      <c r="L3" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="M3" s="13" t="s">
+      <c r="M3" s="10" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:13">
-      <c r="B4" s="15" t="s">
+      <c r="B4" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="25">
+      <c r="C4" s="21">
         <v>76</v>
       </c>
-      <c r="D4" s="26">
+      <c r="D4" s="22">
         <v>80</v>
       </c>
-      <c r="E4" s="10"/>
-      <c r="F4" s="10"/>
-      <c r="G4" s="10"/>
-      <c r="H4" s="10"/>
-      <c r="I4" s="10"/>
-      <c r="J4" s="10"/>
-      <c r="K4" s="10"/>
-      <c r="L4" s="10"/>
-      <c r="M4" s="11"/>
+      <c r="E4" s="22">
+        <v>85</v>
+      </c>
+      <c r="F4" s="7"/>
+      <c r="G4" s="7"/>
+      <c r="H4" s="7"/>
+      <c r="I4" s="7"/>
+      <c r="J4" s="7"/>
+      <c r="K4" s="7"/>
+      <c r="L4" s="7"/>
+      <c r="M4" s="8"/>
     </row>
     <row r="5" spans="1:13">
-      <c r="B5" s="16" t="s">
+      <c r="B5" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="27">
+      <c r="C5" s="23">
         <v>84</v>
       </c>
-      <c r="D5" s="28">
+      <c r="D5" s="24">
         <v>84</v>
       </c>
-      <c r="E5" s="3"/>
+      <c r="E5" s="24">
+        <v>84</v>
+      </c>
       <c r="F5" s="3"/>
       <c r="G5" s="3"/>
       <c r="H5" s="3"/>
@@ -972,16 +985,18 @@
       <c r="M5" s="4"/>
     </row>
     <row r="6" spans="1:13" ht="31.5">
-      <c r="B6" s="17" t="s">
+      <c r="B6" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="21">
+      <c r="C6" s="23">
         <v>87</v>
       </c>
-      <c r="D6" s="22">
+      <c r="D6" s="24">
         <v>87</v>
       </c>
-      <c r="E6" s="3"/>
+      <c r="E6" s="24">
+        <v>87</v>
+      </c>
       <c r="F6" s="3"/>
       <c r="G6" s="3"/>
       <c r="H6" s="3"/>
@@ -992,16 +1007,18 @@
       <c r="M6" s="4"/>
     </row>
     <row r="7" spans="1:13" ht="16.5" thickBot="1">
-      <c r="B7" s="18" t="s">
+      <c r="B7" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="23">
+      <c r="C7" s="35">
         <v>78</v>
       </c>
-      <c r="D7" s="24">
+      <c r="D7" s="36">
         <v>78</v>
       </c>
-      <c r="E7" s="5"/>
+      <c r="E7" s="36">
+        <v>78</v>
+      </c>
       <c r="F7" s="5"/>
       <c r="G7" s="5"/>
       <c r="H7" s="5"/>
@@ -1025,7 +1042,7 @@
   <dimension ref="A1:M7"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75"/>
@@ -1039,88 +1056,92 @@
       <c r="A1" s="1"/>
     </row>
     <row r="2" spans="1:13" ht="16.5" thickBot="1">
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="31" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8"/>
-      <c r="G2" s="8"/>
-      <c r="H2" s="8"/>
-      <c r="I2" s="8"/>
-      <c r="J2" s="8"/>
-      <c r="K2" s="8"/>
-      <c r="L2" s="8"/>
-      <c r="M2" s="9"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="32"/>
+      <c r="G2" s="32"/>
+      <c r="H2" s="32"/>
+      <c r="I2" s="32"/>
+      <c r="J2" s="32"/>
+      <c r="K2" s="32"/>
+      <c r="L2" s="32"/>
+      <c r="M2" s="33"/>
     </row>
     <row r="3" spans="1:13" ht="16.5" thickBot="1">
-      <c r="B3" s="20"/>
-      <c r="C3" s="19" t="s">
+      <c r="B3" s="16"/>
+      <c r="C3" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="12" t="s">
+      <c r="D3" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="12" t="s">
+      <c r="E3" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="F3" s="12" t="s">
+      <c r="F3" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="G3" s="12" t="s">
+      <c r="G3" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="H3" s="12" t="s">
+      <c r="H3" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="I3" s="12" t="s">
+      <c r="I3" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="J3" s="12" t="s">
+      <c r="J3" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="K3" s="12" t="s">
+      <c r="K3" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="L3" s="12" t="s">
+      <c r="L3" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="M3" s="13" t="s">
+      <c r="M3" s="10" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:13">
-      <c r="B4" s="15" t="s">
+      <c r="B4" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="25">
+      <c r="C4" s="21">
         <v>73</v>
       </c>
-      <c r="D4" s="26">
+      <c r="D4" s="22">
         <v>89</v>
       </c>
-      <c r="E4" s="10"/>
-      <c r="F4" s="10"/>
-      <c r="G4" s="10"/>
-      <c r="H4" s="10"/>
-      <c r="I4" s="10"/>
-      <c r="J4" s="10"/>
-      <c r="K4" s="10"/>
-      <c r="L4" s="10"/>
-      <c r="M4" s="11"/>
+      <c r="E4" s="34">
+        <v>90</v>
+      </c>
+      <c r="F4" s="7"/>
+      <c r="G4" s="7"/>
+      <c r="H4" s="7"/>
+      <c r="I4" s="7"/>
+      <c r="J4" s="7"/>
+      <c r="K4" s="7"/>
+      <c r="L4" s="7"/>
+      <c r="M4" s="8"/>
     </row>
     <row r="5" spans="1:13">
-      <c r="B5" s="16" t="s">
+      <c r="B5" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="27">
+      <c r="C5" s="23">
         <v>81</v>
       </c>
-      <c r="D5" s="28">
+      <c r="D5" s="24">
         <v>81</v>
       </c>
-      <c r="E5" s="3"/>
+      <c r="E5" s="24">
+        <v>81</v>
+      </c>
       <c r="F5" s="3"/>
       <c r="G5" s="3"/>
       <c r="H5" s="3"/>
@@ -1131,16 +1152,18 @@
       <c r="M5" s="4"/>
     </row>
     <row r="6" spans="1:13" ht="31.5">
-      <c r="B6" s="17" t="s">
+      <c r="B6" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="21">
+      <c r="C6" s="17">
         <v>93</v>
       </c>
-      <c r="D6" s="22">
+      <c r="D6" s="18">
         <v>93</v>
       </c>
-      <c r="E6" s="3"/>
+      <c r="E6" s="18">
+        <v>93</v>
+      </c>
       <c r="F6" s="3"/>
       <c r="G6" s="3"/>
       <c r="H6" s="3"/>
@@ -1151,16 +1174,18 @@
       <c r="M6" s="4"/>
     </row>
     <row r="7" spans="1:13" ht="16.5" thickBot="1">
-      <c r="B7" s="18" t="s">
+      <c r="B7" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="23">
+      <c r="C7" s="19">
         <v>90</v>
       </c>
-      <c r="D7" s="24">
+      <c r="D7" s="20">
         <v>90</v>
       </c>
-      <c r="E7" s="5"/>
+      <c r="E7" s="20">
+        <v>90</v>
+      </c>
       <c r="F7" s="5"/>
       <c r="G7" s="5"/>
       <c r="H7" s="5"/>
@@ -1183,7 +1208,7 @@
   <dimension ref="A1:M7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+      <selection activeCell="E4" sqref="E4:E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75"/>
@@ -1197,88 +1222,92 @@
       <c r="A1" s="1"/>
     </row>
     <row r="2" spans="1:13" ht="16.5" thickBot="1">
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="31" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8"/>
-      <c r="G2" s="8"/>
-      <c r="H2" s="8"/>
-      <c r="I2" s="8"/>
-      <c r="J2" s="8"/>
-      <c r="K2" s="8"/>
-      <c r="L2" s="8"/>
-      <c r="M2" s="9"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="32"/>
+      <c r="G2" s="32"/>
+      <c r="H2" s="32"/>
+      <c r="I2" s="32"/>
+      <c r="J2" s="32"/>
+      <c r="K2" s="32"/>
+      <c r="L2" s="32"/>
+      <c r="M2" s="33"/>
     </row>
     <row r="3" spans="1:13" ht="16.5" thickBot="1">
-      <c r="B3" s="20"/>
-      <c r="C3" s="19" t="s">
+      <c r="B3" s="16"/>
+      <c r="C3" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="12" t="s">
+      <c r="D3" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="12" t="s">
+      <c r="E3" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="F3" s="12" t="s">
+      <c r="F3" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="G3" s="12" t="s">
+      <c r="G3" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="H3" s="12" t="s">
+      <c r="H3" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="I3" s="12" t="s">
+      <c r="I3" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="J3" s="12" t="s">
+      <c r="J3" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="K3" s="12" t="s">
+      <c r="K3" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="L3" s="12" t="s">
+      <c r="L3" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="M3" s="13" t="s">
+      <c r="M3" s="10" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:13">
-      <c r="B4" s="15" t="s">
+      <c r="B4" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="33">
+      <c r="C4" s="37">
         <v>96</v>
       </c>
-      <c r="D4" s="34">
+      <c r="D4" s="38">
         <v>100</v>
       </c>
-      <c r="E4" s="34"/>
-      <c r="F4" s="34"/>
-      <c r="G4" s="34"/>
-      <c r="H4" s="34"/>
-      <c r="I4" s="34"/>
-      <c r="J4" s="34"/>
-      <c r="K4" s="34"/>
-      <c r="L4" s="34"/>
-      <c r="M4" s="35"/>
+      <c r="E4" s="38">
+        <v>100</v>
+      </c>
+      <c r="F4" s="29"/>
+      <c r="G4" s="29"/>
+      <c r="H4" s="29"/>
+      <c r="I4" s="29"/>
+      <c r="J4" s="29"/>
+      <c r="K4" s="29"/>
+      <c r="L4" s="29"/>
+      <c r="M4" s="30"/>
     </row>
     <row r="5" spans="1:13" ht="16.5" thickBot="1">
-      <c r="B5" s="18" t="s">
+      <c r="B5" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="14">
+      <c r="C5" s="35">
         <v>88</v>
       </c>
-      <c r="D5" s="5">
+      <c r="D5" s="20">
         <v>96</v>
       </c>
-      <c r="E5" s="5"/>
+      <c r="E5" s="20">
+        <v>95</v>
+      </c>
       <c r="F5" s="5"/>
       <c r="G5" s="5"/>
       <c r="H5" s="5"/>
@@ -1288,33 +1317,33 @@
       <c r="L5" s="5"/>
       <c r="M5" s="6"/>
     </row>
-    <row r="6" spans="1:13" s="29" customFormat="1">
-      <c r="B6" s="30"/>
-      <c r="C6" s="31"/>
-      <c r="D6" s="31"/>
-      <c r="E6" s="31"/>
-      <c r="F6" s="31"/>
-      <c r="G6" s="31"/>
-      <c r="H6" s="31"/>
-      <c r="I6" s="31"/>
-      <c r="J6" s="31"/>
-      <c r="K6" s="31"/>
-      <c r="L6" s="31"/>
-      <c r="M6" s="31"/>
-    </row>
-    <row r="7" spans="1:13" s="29" customFormat="1">
-      <c r="B7" s="32"/>
-      <c r="C7" s="31"/>
-      <c r="D7" s="31"/>
-      <c r="E7" s="31"/>
-      <c r="F7" s="31"/>
-      <c r="G7" s="31"/>
-      <c r="H7" s="31"/>
-      <c r="I7" s="31"/>
-      <c r="J7" s="31"/>
-      <c r="K7" s="31"/>
-      <c r="L7" s="31"/>
-      <c r="M7" s="31"/>
+    <row r="6" spans="1:13" s="25" customFormat="1">
+      <c r="B6" s="26"/>
+      <c r="C6" s="27"/>
+      <c r="D6" s="27"/>
+      <c r="E6" s="27"/>
+      <c r="F6" s="27"/>
+      <c r="G6" s="27"/>
+      <c r="H6" s="27"/>
+      <c r="I6" s="27"/>
+      <c r="J6" s="27"/>
+      <c r="K6" s="27"/>
+      <c r="L6" s="27"/>
+      <c r="M6" s="27"/>
+    </row>
+    <row r="7" spans="1:13" s="25" customFormat="1">
+      <c r="B7" s="28"/>
+      <c r="C7" s="27"/>
+      <c r="D7" s="27"/>
+      <c r="E7" s="27"/>
+      <c r="F7" s="27"/>
+      <c r="G7" s="27"/>
+      <c r="H7" s="27"/>
+      <c r="I7" s="27"/>
+      <c r="J7" s="27"/>
+      <c r="K7" s="27"/>
+      <c r="L7" s="27"/>
+      <c r="M7" s="27"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Analyses des performances après 2ème correction
</commit_message>
<xml_diff>
--- a/Analyses/Évolution.xlsx
+++ b/Analyses/Évolution.xlsx
@@ -554,6 +554,21 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -561,21 +576,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -875,7 +875,7 @@
   <dimension ref="A1:M7"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4:E7"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75"/>
@@ -889,20 +889,20 @@
       <c r="A1" s="1"/>
     </row>
     <row r="2" spans="1:13" ht="16.5" thickBot="1">
-      <c r="B2" s="31" t="s">
+      <c r="B2" s="36" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="32"/>
-      <c r="D2" s="32"/>
-      <c r="E2" s="32"/>
-      <c r="F2" s="32"/>
-      <c r="G2" s="32"/>
-      <c r="H2" s="32"/>
-      <c r="I2" s="32"/>
-      <c r="J2" s="32"/>
-      <c r="K2" s="32"/>
-      <c r="L2" s="32"/>
-      <c r="M2" s="33"/>
+      <c r="C2" s="37"/>
+      <c r="D2" s="37"/>
+      <c r="E2" s="37"/>
+      <c r="F2" s="37"/>
+      <c r="G2" s="37"/>
+      <c r="H2" s="37"/>
+      <c r="I2" s="37"/>
+      <c r="J2" s="37"/>
+      <c r="K2" s="37"/>
+      <c r="L2" s="37"/>
+      <c r="M2" s="38"/>
     </row>
     <row r="3" spans="1:13" ht="16.5" thickBot="1">
       <c r="B3" s="16"/>
@@ -951,7 +951,7 @@
         <v>80</v>
       </c>
       <c r="E4" s="22">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="F4" s="7"/>
       <c r="G4" s="7"/>
@@ -1010,13 +1010,13 @@
       <c r="B7" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="35">
+      <c r="C7" s="32">
         <v>78</v>
       </c>
-      <c r="D7" s="36">
+      <c r="D7" s="33">
         <v>78</v>
       </c>
-      <c r="E7" s="36">
+      <c r="E7" s="33">
         <v>78</v>
       </c>
       <c r="F7" s="5"/>
@@ -1042,7 +1042,7 @@
   <dimension ref="A1:M7"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75"/>
@@ -1056,20 +1056,20 @@
       <c r="A1" s="1"/>
     </row>
     <row r="2" spans="1:13" ht="16.5" thickBot="1">
-      <c r="B2" s="31" t="s">
+      <c r="B2" s="36" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="32"/>
-      <c r="D2" s="32"/>
-      <c r="E2" s="32"/>
-      <c r="F2" s="32"/>
-      <c r="G2" s="32"/>
-      <c r="H2" s="32"/>
-      <c r="I2" s="32"/>
-      <c r="J2" s="32"/>
-      <c r="K2" s="32"/>
-      <c r="L2" s="32"/>
-      <c r="M2" s="33"/>
+      <c r="C2" s="37"/>
+      <c r="D2" s="37"/>
+      <c r="E2" s="37"/>
+      <c r="F2" s="37"/>
+      <c r="G2" s="37"/>
+      <c r="H2" s="37"/>
+      <c r="I2" s="37"/>
+      <c r="J2" s="37"/>
+      <c r="K2" s="37"/>
+      <c r="L2" s="37"/>
+      <c r="M2" s="38"/>
     </row>
     <row r="3" spans="1:13" ht="16.5" thickBot="1">
       <c r="B3" s="16"/>
@@ -1117,8 +1117,8 @@
       <c r="D4" s="22">
         <v>89</v>
       </c>
-      <c r="E4" s="34">
-        <v>90</v>
+      <c r="E4" s="31">
+        <v>92</v>
       </c>
       <c r="F4" s="7"/>
       <c r="G4" s="7"/>
@@ -1208,7 +1208,7 @@
   <dimension ref="A1:M7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4:E5"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75"/>
@@ -1222,20 +1222,20 @@
       <c r="A1" s="1"/>
     </row>
     <row r="2" spans="1:13" ht="16.5" thickBot="1">
-      <c r="B2" s="31" t="s">
+      <c r="B2" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="32"/>
-      <c r="D2" s="32"/>
-      <c r="E2" s="32"/>
-      <c r="F2" s="32"/>
-      <c r="G2" s="32"/>
-      <c r="H2" s="32"/>
-      <c r="I2" s="32"/>
-      <c r="J2" s="32"/>
-      <c r="K2" s="32"/>
-      <c r="L2" s="32"/>
-      <c r="M2" s="33"/>
+      <c r="C2" s="37"/>
+      <c r="D2" s="37"/>
+      <c r="E2" s="37"/>
+      <c r="F2" s="37"/>
+      <c r="G2" s="37"/>
+      <c r="H2" s="37"/>
+      <c r="I2" s="37"/>
+      <c r="J2" s="37"/>
+      <c r="K2" s="37"/>
+      <c r="L2" s="37"/>
+      <c r="M2" s="38"/>
     </row>
     <row r="3" spans="1:13" ht="16.5" thickBot="1">
       <c r="B3" s="16"/>
@@ -1277,13 +1277,13 @@
       <c r="B4" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="37">
+      <c r="C4" s="34">
         <v>96</v>
       </c>
-      <c r="D4" s="38">
+      <c r="D4" s="35">
         <v>100</v>
       </c>
-      <c r="E4" s="38">
+      <c r="E4" s="35">
         <v>100</v>
       </c>
       <c r="F4" s="29"/>
@@ -1299,14 +1299,14 @@
       <c r="B5" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="35">
+      <c r="C5" s="32">
         <v>88</v>
       </c>
       <c r="D5" s="20">
         <v>96</v>
       </c>
       <c r="E5" s="20">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="F5" s="5"/>
       <c r="G5" s="5"/>

</xml_diff>

<commit_message>
Analyses des performances après 3ème correction
</commit_message>
<xml_diff>
--- a/Analyses/Évolution.xlsx
+++ b/Analyses/Évolution.xlsx
@@ -462,7 +462,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -576,6 +576,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -875,7 +878,7 @@
   <dimension ref="A1:M7"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="F4" sqref="F4:F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75"/>
@@ -953,7 +956,9 @@
       <c r="E4" s="22">
         <v>83</v>
       </c>
-      <c r="F4" s="7"/>
+      <c r="F4" s="22">
+        <v>89</v>
+      </c>
       <c r="G4" s="7"/>
       <c r="H4" s="7"/>
       <c r="I4" s="7"/>
@@ -975,7 +980,9 @@
       <c r="E5" s="24">
         <v>84</v>
       </c>
-      <c r="F5" s="3"/>
+      <c r="F5" s="24">
+        <v>88</v>
+      </c>
       <c r="G5" s="3"/>
       <c r="H5" s="3"/>
       <c r="I5" s="3"/>
@@ -997,7 +1004,9 @@
       <c r="E6" s="24">
         <v>87</v>
       </c>
-      <c r="F6" s="3"/>
+      <c r="F6" s="24">
+        <v>87</v>
+      </c>
       <c r="G6" s="3"/>
       <c r="H6" s="3"/>
       <c r="I6" s="3"/>
@@ -1019,7 +1028,9 @@
       <c r="E7" s="33">
         <v>78</v>
       </c>
-      <c r="F7" s="5"/>
+      <c r="F7" s="33">
+        <v>78</v>
+      </c>
       <c r="G7" s="5"/>
       <c r="H7" s="5"/>
       <c r="I7" s="5"/>
@@ -1042,7 +1053,7 @@
   <dimension ref="A1:M7"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="E36" sqref="E36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75"/>
@@ -1120,7 +1131,9 @@
       <c r="E4" s="31">
         <v>92</v>
       </c>
-      <c r="F4" s="7"/>
+      <c r="F4" s="31">
+        <v>90</v>
+      </c>
       <c r="G4" s="7"/>
       <c r="H4" s="7"/>
       <c r="I4" s="7"/>
@@ -1142,7 +1155,9 @@
       <c r="E5" s="24">
         <v>81</v>
       </c>
-      <c r="F5" s="3"/>
+      <c r="F5" s="24">
+        <v>86</v>
+      </c>
       <c r="G5" s="3"/>
       <c r="H5" s="3"/>
       <c r="I5" s="3"/>
@@ -1164,7 +1179,9 @@
       <c r="E6" s="18">
         <v>93</v>
       </c>
-      <c r="F6" s="3"/>
+      <c r="F6" s="18">
+        <v>93</v>
+      </c>
       <c r="G6" s="3"/>
       <c r="H6" s="3"/>
       <c r="I6" s="3"/>
@@ -1186,7 +1203,9 @@
       <c r="E7" s="20">
         <v>90</v>
       </c>
-      <c r="F7" s="5"/>
+      <c r="F7" s="20">
+        <v>90</v>
+      </c>
       <c r="G7" s="5"/>
       <c r="H7" s="5"/>
       <c r="I7" s="5"/>
@@ -1205,10 +1224,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M7"/>
+  <dimension ref="A1:M12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75"/>
@@ -1286,7 +1305,9 @@
       <c r="E4" s="35">
         <v>100</v>
       </c>
-      <c r="F4" s="29"/>
+      <c r="F4" s="35">
+        <v>97</v>
+      </c>
       <c r="G4" s="29"/>
       <c r="H4" s="29"/>
       <c r="I4" s="29"/>
@@ -1308,7 +1329,9 @@
       <c r="E5" s="20">
         <v>96</v>
       </c>
-      <c r="F5" s="5"/>
+      <c r="F5" s="20">
+        <v>94</v>
+      </c>
       <c r="G5" s="5"/>
       <c r="H5" s="5"/>
       <c r="I5" s="5"/>
@@ -1345,6 +1368,9 @@
       <c r="L7" s="27"/>
       <c r="M7" s="27"/>
     </row>
+    <row r="12" spans="1:13">
+      <c r="I12" s="39"/>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B2:M2"/>

</xml_diff>

<commit_message>
Analyses des performances apres 7eme correction
</commit_message>
<xml_diff>
--- a/Analyses/Évolution.xlsx
+++ b/Analyses/Évolution.xlsx
@@ -878,7 +878,7 @@
   <dimension ref="A1:M7"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4:J7"/>
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75"/>
@@ -969,7 +969,7 @@
         <v>82</v>
       </c>
       <c r="J4" s="22">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="K4" s="7"/>
       <c r="L4" s="7"/>
@@ -1175,8 +1175,8 @@
       <c r="I4" s="22">
         <v>88</v>
       </c>
-      <c r="J4" s="22">
-        <v>89</v>
+      <c r="J4" s="31">
+        <v>90</v>
       </c>
       <c r="K4" s="7"/>
       <c r="L4" s="7"/>
@@ -1291,7 +1291,7 @@
   <dimension ref="A1:M12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J4" sqref="J4:J5"/>
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75"/>
@@ -1382,7 +1382,7 @@
         <v>100</v>
       </c>
       <c r="J4" s="35">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="K4" s="29"/>
       <c r="L4" s="29"/>
@@ -1414,7 +1414,7 @@
         <v>96</v>
       </c>
       <c r="J5" s="20">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="K5" s="5"/>
       <c r="L5" s="5"/>

</xml_diff>